<commit_message>
Nueva versión para sacar ggrafos y nuevas visualizaciones
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -5,652 +5,660 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="145" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$67</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="212">
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>libro</t>
-  </si>
-  <si>
-    <t>testamento</t>
-  </si>
-  <si>
-    <t>hecho</t>
-  </si>
-  <si>
-    <t>english</t>
-  </si>
-  <si>
-    <t>codebook</t>
-  </si>
-  <si>
-    <t>Chapters</t>
-  </si>
-  <si>
-    <t>Genre</t>
-  </si>
-  <si>
-    <t>Génesis</t>
-  </si>
-  <si>
-    <t>antiguo</t>
-  </si>
-  <si>
-    <t>Genesis</t>
-  </si>
-  <si>
-    <t>GEN</t>
-  </si>
-  <si>
-    <t>historical</t>
-  </si>
-  <si>
-    <t>Éxodo</t>
-  </si>
-  <si>
-    <t>Exodus</t>
-  </si>
-  <si>
-    <t>EXO</t>
-  </si>
-  <si>
-    <t>Levítico</t>
-  </si>
-  <si>
-    <t>Leviticus</t>
-  </si>
-  <si>
-    <t>LEV</t>
-  </si>
-  <si>
-    <t>law</t>
-  </si>
-  <si>
-    <t>Números</t>
-  </si>
-  <si>
-    <t>Numbers</t>
-  </si>
-  <si>
-    <t>NUM</t>
-  </si>
-  <si>
-    <t>Deuteronomio</t>
-  </si>
-  <si>
-    <t>Deuteronomy</t>
-  </si>
-  <si>
-    <t>DEU</t>
-  </si>
-  <si>
-    <t>Josué</t>
-  </si>
-  <si>
-    <t>Joshua</t>
-  </si>
-  <si>
-    <t>JOS</t>
-  </si>
-  <si>
-    <t>Jueces</t>
-  </si>
-  <si>
-    <t>Judges</t>
-  </si>
-  <si>
-    <t>JDG</t>
-  </si>
-  <si>
-    <t>Rut</t>
-  </si>
-  <si>
-    <t>Ruth</t>
-  </si>
-  <si>
-    <t>RUT</t>
-  </si>
-  <si>
-    <t>1 Samuel</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>1SA</t>
-  </si>
-  <si>
-    <t>2 Samuel</t>
-  </si>
-  <si>
-    <t>2SA</t>
-  </si>
-  <si>
-    <t>1 Reyes</t>
-  </si>
-  <si>
-    <t>1 Kings</t>
-  </si>
-  <si>
-    <t>1KI</t>
-  </si>
-  <si>
-    <t>2 Reyes</t>
-  </si>
-  <si>
-    <t>2 Kings</t>
-  </si>
-  <si>
-    <t>2KI</t>
-  </si>
-  <si>
-    <t>1 Crónicas</t>
-  </si>
-  <si>
-    <t>1 Chronicles</t>
-  </si>
-  <si>
-    <t>1CH</t>
-  </si>
-  <si>
-    <t>2 Crónicas</t>
-  </si>
-  <si>
-    <t>2 Chronicles</t>
-  </si>
-  <si>
-    <t>2CH</t>
-  </si>
-  <si>
-    <t>Esdras</t>
-  </si>
-  <si>
-    <t>Ezra</t>
-  </si>
-  <si>
-    <t>EZR</t>
-  </si>
-  <si>
-    <t>Nehemías</t>
-  </si>
-  <si>
-    <t>Nehemiah</t>
-  </si>
-  <si>
-    <t>NEH</t>
-  </si>
-  <si>
-    <t>Ester</t>
-  </si>
-  <si>
-    <t>Esther</t>
-  </si>
-  <si>
-    <t>EST</t>
-  </si>
-  <si>
-    <t>Job</t>
-  </si>
-  <si>
-    <t>JOB</t>
-  </si>
-  <si>
-    <t>wisdom</t>
-  </si>
-  <si>
-    <t>Salmos</t>
-  </si>
-  <si>
-    <t>Psalms</t>
-  </si>
-  <si>
-    <t>PSA</t>
-  </si>
-  <si>
-    <t>lyric</t>
-  </si>
-  <si>
-    <t>Proverbios</t>
-  </si>
-  <si>
-    <t>Proverbs</t>
-  </si>
-  <si>
-    <t>PRO</t>
-  </si>
-  <si>
-    <t>Eclesiastés</t>
-  </si>
-  <si>
-    <t>Ecclesiastes</t>
-  </si>
-  <si>
-    <t>ECC</t>
-  </si>
-  <si>
-    <t>Cantares</t>
-  </si>
-  <si>
-    <t>Song of Solomon</t>
-  </si>
-  <si>
-    <t>SON</t>
-  </si>
-  <si>
-    <t>Isaías</t>
-  </si>
-  <si>
-    <t>Isaiah</t>
-  </si>
-  <si>
-    <t>ISA</t>
-  </si>
-  <si>
-    <t>apocalyptic</t>
-  </si>
-  <si>
-    <t>Jeremías</t>
-  </si>
-  <si>
-    <t>Jeremiah</t>
-  </si>
-  <si>
-    <t>JER</t>
-  </si>
-  <si>
-    <t>prophecy</t>
-  </si>
-  <si>
-    <t>Lamentaciones</t>
-  </si>
-  <si>
-    <t>Lamentations</t>
-  </si>
-  <si>
-    <t>LAM</t>
-  </si>
-  <si>
-    <t>Ezequiel</t>
-  </si>
-  <si>
-    <t>Ezekiel</t>
-  </si>
-  <si>
-    <t>EZE</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>DAN</t>
-  </si>
-  <si>
-    <t>Oseas</t>
-  </si>
-  <si>
-    <t>Hosea</t>
-  </si>
-  <si>
-    <t>HOS</t>
-  </si>
-  <si>
-    <t>Joel</t>
-  </si>
-  <si>
-    <t>JOE</t>
-  </si>
-  <si>
-    <t>Amós</t>
-  </si>
-  <si>
-    <t>Amos</t>
-  </si>
-  <si>
-    <t>AMO</t>
-  </si>
-  <si>
-    <t>Abdías</t>
-  </si>
-  <si>
-    <t>Obadiah</t>
-  </si>
-  <si>
-    <t>OBA</t>
-  </si>
-  <si>
-    <t>Jonás</t>
-  </si>
-  <si>
-    <t>Jonah</t>
-  </si>
-  <si>
-    <t>JON</t>
-  </si>
-  <si>
-    <t>Miqueas</t>
-  </si>
-  <si>
-    <t>Micah</t>
-  </si>
-  <si>
-    <t>MIC</t>
-  </si>
-  <si>
-    <t>Nahúm</t>
-  </si>
-  <si>
-    <t>Nahum</t>
-  </si>
-  <si>
-    <t>NAH</t>
-  </si>
-  <si>
-    <t>Habacuc</t>
-  </si>
-  <si>
-    <t>Habakkuk</t>
-  </si>
-  <si>
-    <t>HAB</t>
-  </si>
-  <si>
-    <t>Sofonías</t>
-  </si>
-  <si>
-    <t>Zephaniah</t>
-  </si>
-  <si>
-    <t>ZEP</t>
-  </si>
-  <si>
-    <t>Hageo</t>
-  </si>
-  <si>
-    <t>Haggai</t>
-  </si>
-  <si>
-    <t>HAG</t>
-  </si>
-  <si>
-    <t>Zacarías</t>
-  </si>
-  <si>
-    <t>Zechariah</t>
-  </si>
-  <si>
-    <t>ZEC</t>
-  </si>
-  <si>
-    <t>Malaquías</t>
-  </si>
-  <si>
-    <t>Malachi</t>
-  </si>
-  <si>
-    <t>MAL</t>
-  </si>
-  <si>
-    <t>Mateo</t>
-  </si>
-  <si>
-    <t>nuevo</t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>MAT</t>
-  </si>
-  <si>
-    <t>Gospel</t>
-  </si>
-  <si>
-    <t>Marcos</t>
-  </si>
-  <si>
-    <t>Mark</t>
-  </si>
-  <si>
-    <t>MAR</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
-    <t>Luke</t>
-  </si>
-  <si>
-    <t>LUK</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>JOH</t>
-  </si>
-  <si>
-    <t>Hechos</t>
-  </si>
-  <si>
-    <t>Acts</t>
-  </si>
-  <si>
-    <t>ACT</t>
-  </si>
-  <si>
-    <t>Romanos</t>
-  </si>
-  <si>
-    <t>Romans</t>
-  </si>
-  <si>
-    <t>ROM</t>
-  </si>
-  <si>
-    <t>letter</t>
-  </si>
-  <si>
-    <t>1 Corintios</t>
-  </si>
-  <si>
-    <t>1 Corinthians</t>
-  </si>
-  <si>
-    <t>1CO</t>
-  </si>
-  <si>
-    <t>2 Corintios</t>
-  </si>
-  <si>
-    <t>2 Corinthians</t>
-  </si>
-  <si>
-    <t>2CO</t>
-  </si>
-  <si>
-    <t>Gálatas</t>
-  </si>
-  <si>
-    <t>Galatians</t>
-  </si>
-  <si>
-    <t>GAL</t>
-  </si>
-  <si>
-    <t>Efesios</t>
-  </si>
-  <si>
-    <t>Ephesians</t>
-  </si>
-  <si>
-    <t>EPH</t>
-  </si>
-  <si>
-    <t>Filipenses</t>
-  </si>
-  <si>
-    <t>Philippians</t>
-  </si>
-  <si>
-    <t>PHI</t>
-  </si>
-  <si>
-    <t>Colosenses</t>
-  </si>
-  <si>
-    <t>Colossians</t>
-  </si>
-  <si>
-    <t>COL</t>
-  </si>
-  <si>
-    <t>1 Tesalonicenses</t>
-  </si>
-  <si>
-    <t>1 Thessalonians</t>
-  </si>
-  <si>
-    <t>1TH</t>
-  </si>
-  <si>
-    <t>2 Tesalonicenses</t>
-  </si>
-  <si>
-    <t>2 Thessalonians</t>
-  </si>
-  <si>
-    <t>2TH</t>
-  </si>
-  <si>
-    <t>1 Timoteo</t>
-  </si>
-  <si>
-    <t>1 Timothy</t>
-  </si>
-  <si>
-    <t>1TI</t>
-  </si>
-  <si>
-    <t>2 Timoteo</t>
-  </si>
-  <si>
-    <t>2 Timothy</t>
-  </si>
-  <si>
-    <t>2TI</t>
-  </si>
-  <si>
-    <t>Tito</t>
-  </si>
-  <si>
-    <t>Titus</t>
-  </si>
-  <si>
-    <t>TIT</t>
-  </si>
-  <si>
-    <t>Filemón</t>
-  </si>
-  <si>
-    <t>Philemon</t>
-  </si>
-  <si>
-    <t>PHM</t>
-  </si>
-  <si>
-    <t>Hebreos</t>
-  </si>
-  <si>
-    <t>Hebrews</t>
-  </si>
-  <si>
-    <t>HEB</t>
-  </si>
-  <si>
-    <t>Santiago</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>JAM</t>
-  </si>
-  <si>
-    <t>1 Pedro</t>
-  </si>
-  <si>
-    <t>1 Peter</t>
-  </si>
-  <si>
-    <t>1PE</t>
-  </si>
-  <si>
-    <t>2 Pedro</t>
-  </si>
-  <si>
-    <t>2 Peter</t>
-  </si>
-  <si>
-    <t>2PE</t>
-  </si>
-  <si>
-    <t>1 Juan</t>
-  </si>
-  <si>
-    <t>1 John</t>
-  </si>
-  <si>
-    <t>1JO</t>
-  </si>
-  <si>
-    <t>2 Juan</t>
-  </si>
-  <si>
-    <t>2 John</t>
-  </si>
-  <si>
-    <t>2JO</t>
-  </si>
-  <si>
-    <t>3 Juan</t>
-  </si>
-  <si>
-    <t>3 John</t>
-  </si>
-  <si>
-    <t>3JO</t>
-  </si>
-  <si>
-    <t>Judas</t>
-  </si>
-  <si>
-    <t>Jude</t>
-  </si>
-  <si>
-    <t>JUD</t>
-  </si>
-  <si>
-    <t>Apocalipsis</t>
-  </si>
-  <si>
-    <t>Revelation</t>
-  </si>
-  <si>
-    <t>REV</t>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hecho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">codebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chapters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Génesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antiguo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">historical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Éxodo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exodus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Levítico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leviticus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">law</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Números</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deuteronomio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deuteronomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josué</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jueces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Samuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Samuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Reyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Kings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1KI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Reyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Kings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2KI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Crónicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Chronicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Crónicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Chronicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esdras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ezra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EZR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nehemías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nehemiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wisdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psalms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lyric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proverbios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proverbs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eclesiastés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecclesiastes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Song of Solomon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apocalyptic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeremías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeremiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prophecy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lamentaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lamentations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ezequiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ezekiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oseas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hosea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amós</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obadiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miqueas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nahúm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nahum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habacuc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habakkuk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofonías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zephaniah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hageo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haggai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zacarías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zechariah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malaquías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malachi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mateo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuevo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matthew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gospel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hechos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romanos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Corintios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Corinthians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Corintios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Corinthians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gálatas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galatians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efesios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ephesians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filipenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philippians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colosenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colossians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Tesalonicenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Thessalonians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1TH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Tesalonicenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Thessalonians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2TH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Timoteo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Timothy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1TI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Timoteo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Timothy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2TI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filemón</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hebreos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hebrews</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santiago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Pedro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Peter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1PE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Pedro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Peter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2PE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Juan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1JO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Juan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2JO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Juan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3JO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apocalipsis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revelation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REV</t>
   </si>
 </sst>
 </file>
@@ -658,13 +666,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -681,16 +690,139 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -698,8 +830,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -723,22 +870,154 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -748,38 +1027,38 @@
   </sheetPr>
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.85" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2356,12 +2635,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H67"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1 Samuel terminado e integrado
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="212">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -133,13 +134,13 @@
     <t xml:space="preserve">1 Samuel</t>
   </si>
   <si>
+    <t xml:space="preserve">1SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Samuel</t>
+  </si>
+  <si>
     <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1SA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Samuel</t>
   </si>
   <si>
     <t xml:space="preserve">2SA</t>
@@ -1027,8 +1028,8 @@
   </sheetPr>
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D71" activeCellId="0" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1265,14 +1266,14 @@
       <c r="C10" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>36</v>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>31</v>
@@ -1286,16 +1287,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="E11" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>39</v>
@@ -2027,7 +2028,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
@@ -2036,9 +2037,6 @@
       </c>
       <c r="C42" s="0" t="s">
         <v>129</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>1</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>134</v>
@@ -2085,6 +2083,9 @@
       </c>
       <c r="C44" s="0" t="s">
         <v>129</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E44" s="0" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
Empezando con JOB, corregido hasta capítulo 7
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="214">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -622,9 +623,6 @@
     <t xml:space="preserve">1 Juan</t>
   </si>
   <si>
-    <t xml:space="preserve">*</t>
-  </si>
-  <si>
     <t xml:space="preserve">1 John</t>
   </si>
   <si>
@@ -665,6 +663,12 @@
   </si>
   <si>
     <t xml:space="preserve">REV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proportion</t>
   </si>
 </sst>
 </file>
@@ -674,7 +678,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -776,6 +780,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -925,12 +934,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1031,10 +1044,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2721,14 +2734,14 @@
       <c r="D63" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E63" s="0" t="s">
+      <c r="E63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="F63" s="0" t="s">
+      <c r="G63" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="G63" s="0" t="s">
-        <v>200</v>
       </c>
       <c r="H63" s="0" t="n">
         <v>5</v>
@@ -2745,19 +2758,19 @@
         <v>63</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E64" s="0" t="s">
-        <v>198</v>
+      <c r="E64" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F64" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="G64" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="G64" s="0" t="s">
-        <v>203</v>
       </c>
       <c r="H64" s="0" t="n">
         <v>1</v>
@@ -2774,19 +2787,19 @@
         <v>64</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E65" s="0" t="s">
-        <v>198</v>
+      <c r="E65" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F65" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="G65" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="G65" s="0" t="s">
-        <v>206</v>
       </c>
       <c r="H65" s="0" t="n">
         <v>1</v>
@@ -2803,19 +2816,19 @@
         <v>65</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E66" s="0" t="s">
-        <v>198</v>
+      <c r="E66" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F66" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G66" s="0" t="s">
         <v>208</v>
-      </c>
-      <c r="G66" s="0" t="s">
-        <v>209</v>
       </c>
       <c r="H66" s="0" t="n">
         <v>1</v>
@@ -2832,7 +2845,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>129</v>
@@ -2841,16 +2854,51 @@
         <v>1</v>
       </c>
       <c r="F67" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="G67" s="0" t="s">
         <v>211</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>212</v>
       </c>
       <c r="H67" s="0" t="n">
         <v>22</v>
       </c>
       <c r="I67" s="0" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <f aca="false">SUM(H2:H67)</f>
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D69" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E67,1)</f>
+        <v>21</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <f aca="false">SUMIF(E2:E67,1,H2:H67)+75</f>
+        <v>371</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D70" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <f aca="false">E69/E68</f>
+        <v>0.318181818181818</v>
+      </c>
+      <c r="H70" s="0" t="n">
+        <f aca="false">H69/H68</f>
+        <v>0.312026913372582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Job terminado e integrado en archivo principal
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -678,7 +679,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -780,11 +781,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -934,16 +930,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1046,8 +1038,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1554,6 +1546,9 @@
       <c r="D19" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="F19" s="0" t="s">
         <v>61</v>
       </c>
@@ -2881,11 +2876,11 @@
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">COUNTIF(E2:E67,1)</f>
-        <v>21</v>
-      </c>
-      <c r="H69" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="H69" s="1" t="n">
         <f aca="false">SUMIF(E2:E67,1,H2:H67)+75</f>
-        <v>371</v>
+        <v>413</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2894,11 +2889,11 @@
       </c>
       <c r="E70" s="0" t="n">
         <f aca="false">E69/E68</f>
-        <v>0.318181818181818</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="H70" s="0" t="n">
         <f aca="false">H69/H68</f>
-        <v>0.312026913372582</v>
+        <v>0.347350714886459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Empezando nuevas cartas y primer capítulo de Santiago
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -17,6 +17,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="215">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -595,6 +596,9 @@
   </si>
   <si>
     <t xml:space="preserve">Santiago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">James</t>
@@ -1038,8 +1042,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H68" activeCellId="0" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2651,11 +2655,14 @@
       <c r="D60" s="0" t="s">
         <v>129</v>
       </c>
+      <c r="E60" s="0" t="s">
+        <v>189</v>
+      </c>
       <c r="F60" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H60" s="0" t="n">
         <v>5</v>
@@ -2672,16 +2679,19 @@
         <v>60</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>129</v>
       </c>
+      <c r="E61" s="0" t="s">
+        <v>189</v>
+      </c>
       <c r="F61" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H61" s="0" t="n">
         <v>5</v>
@@ -2698,16 +2708,19 @@
         <v>61</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>129</v>
       </c>
+      <c r="E62" s="0" t="s">
+        <v>189</v>
+      </c>
       <c r="F62" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H62" s="0" t="n">
         <v>3</v>
@@ -2724,7 +2737,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>129</v>
@@ -2733,10 +2746,10 @@
         <v>1</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H63" s="0" t="n">
         <v>5</v>
@@ -2753,7 +2766,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>129</v>
@@ -2762,10 +2775,10 @@
         <v>1</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H64" s="0" t="n">
         <v>1</v>
@@ -2782,7 +2795,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>129</v>
@@ -2791,10 +2804,10 @@
         <v>1</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H65" s="0" t="n">
         <v>1</v>
@@ -2811,7 +2824,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>129</v>
@@ -2820,10 +2833,10 @@
         <v>1</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H66" s="0" t="n">
         <v>1</v>
@@ -2840,7 +2853,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>129</v>
@@ -2849,10 +2862,10 @@
         <v>1</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H67" s="0" t="n">
         <v>22</v>
@@ -2872,7 +2885,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D69" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">COUNTIF(E2:E67,1)</f>
@@ -2885,7 +2898,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D70" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E70" s="0" t="n">
         <f aca="false">E69/E68</f>

</xml_diff>

<commit_message>
Terminados Santiago, 1 Pedro y 2 Pedro y libros integrados en archivo principal
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="215">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -298,6 +299,9 @@
     <t xml:space="preserve">Ezequiel</t>
   </si>
   <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ezekiel</t>
   </si>
   <si>
@@ -596,9 +600,6 @@
   </si>
   <si>
     <t xml:space="preserve">Santiago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">James</t>
@@ -1042,8 +1043,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H68" activeCellId="0" sqref="H68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1764,11 +1765,14 @@
       <c r="D27" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E27" s="0" t="s">
+        <v>89</v>
+      </c>
       <c r="F27" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>48</v>
@@ -1785,16 +1789,16 @@
         <v>27</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>12</v>
@@ -1811,16 +1815,16 @@
         <v>28</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>14</v>
@@ -1837,16 +1841,16 @@
         <v>29</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>3</v>
@@ -1863,16 +1867,16 @@
         <v>30</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>9</v>
@@ -1889,16 +1893,16 @@
         <v>31</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>1</v>
@@ -1915,7 +1919,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>10</v>
@@ -1924,10 +1928,10 @@
         <v>1</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>4</v>
@@ -1944,7 +1948,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>10</v>
@@ -1953,10 +1957,10 @@
         <v>1</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>7</v>
@@ -1973,7 +1977,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>10</v>
@@ -1982,10 +1986,10 @@
         <v>1</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>3</v>
@@ -2002,7 +2006,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>10</v>
@@ -2011,10 +2015,10 @@
         <v>1</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>3</v>
@@ -2031,7 +2035,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>10</v>
@@ -2040,10 +2044,10 @@
         <v>1</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>3</v>
@@ -2060,7 +2064,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>10</v>
@@ -2069,10 +2073,10 @@
         <v>1</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>2</v>
@@ -2089,7 +2093,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>10</v>
@@ -2098,10 +2102,10 @@
         <v>1</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>14</v>
@@ -2118,7 +2122,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>10</v>
@@ -2127,10 +2131,10 @@
         <v>1</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>4</v>
@@ -2147,25 +2151,25 @@
         <v>40</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>28</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,22 +2180,22 @@
         <v>41</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H42" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2202,22 +2206,22 @@
         <v>42</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H43" s="0" t="n">
         <v>24</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2228,25 +2232,25 @@
         <v>43</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H44" s="0" t="n">
         <v>21</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2257,25 +2261,25 @@
         <v>44</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H45" s="0" t="n">
         <v>28</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,22 +2290,22 @@
         <v>45</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H46" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2312,22 +2316,22 @@
         <v>46</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H47" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,22 +2342,22 @@
         <v>47</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H48" s="0" t="n">
         <v>13</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,22 +2368,22 @@
         <v>48</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H49" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2390,22 +2394,22 @@
         <v>49</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H50" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2416,22 +2420,22 @@
         <v>50</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H51" s="0" t="n">
         <v>4</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2442,22 +2446,22 @@
         <v>51</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H52" s="0" t="n">
         <v>4</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2468,22 +2472,22 @@
         <v>52</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H53" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2494,22 +2498,22 @@
         <v>53</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H54" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,22 +2524,22 @@
         <v>54</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H55" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,22 +2550,22 @@
         <v>55</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H56" s="0" t="n">
         <v>4</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,22 +2576,22 @@
         <v>56</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H57" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,22 +2602,22 @@
         <v>57</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H58" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2624,22 +2628,22 @@
         <v>58</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H59" s="0" t="n">
         <v>13</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2650,13 +2654,13 @@
         <v>59</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>189</v>
+        <v>130</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F60" s="0" t="s">
         <v>190</v>
@@ -2668,7 +2672,7 @@
         <v>5</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,10 +2686,10 @@
         <v>192</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>189</v>
+        <v>130</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F61" s="0" t="s">
         <v>193</v>
@@ -2697,7 +2701,7 @@
         <v>5</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2711,10 +2715,10 @@
         <v>195</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>189</v>
+        <v>130</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F62" s="0" t="s">
         <v>196</v>
@@ -2726,7 +2730,7 @@
         <v>3</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2740,7 +2744,7 @@
         <v>198</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>1</v>
@@ -2755,7 +2759,7 @@
         <v>5</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2769,7 +2773,7 @@
         <v>201</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>1</v>
@@ -2784,7 +2788,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,7 +2802,7 @@
         <v>204</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>1</v>
@@ -2813,7 +2817,7 @@
         <v>1</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2827,7 +2831,7 @@
         <v>207</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>1</v>
@@ -2842,7 +2846,7 @@
         <v>1</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2856,7 +2860,7 @@
         <v>210</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>1</v>
@@ -2889,11 +2893,11 @@
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">COUNTIF(E2:E67,1)</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H69" s="1" t="n">
         <f aca="false">SUMIF(E2:E67,1,H2:H67)+75</f>
-        <v>413</v>
+        <v>426</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2902,15 +2906,15 @@
       </c>
       <c r="E70" s="0" t="n">
         <f aca="false">E69/E68</f>
-        <v>0.333333333333333</v>
+        <v>0.378787878787879</v>
       </c>
       <c r="H70" s="0" t="n">
         <f aca="false">H69/H68</f>
-        <v>0.347350714886459</v>
+        <v>0.358284272497897</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:I67"/>
+  <autoFilter ref="B1:I70"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Comenzando Ezekiel, primer capítulo corregido
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -11,14 +11,15 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -1043,8 +1044,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2914,7 +2915,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:I70"/>
+  <autoFilter ref="B1:I67"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
1CO integrado en archivo general
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -14,17 +14,18 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="215">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -488,16 +489,16 @@
     <t xml:space="preserve">1 Corintios</t>
   </si>
   <si>
+    <t xml:space="preserve">1 Corinthians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Corintios</t>
+  </si>
+  <si>
     <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Corinthians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Corintios</t>
   </si>
   <si>
     <t xml:space="preserve">2 Corinthians</t>
@@ -1049,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2333,14 +2334,14 @@
       <c r="D47" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="G47" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>152</v>
       </c>
       <c r="H47" s="0" t="n">
         <v>16</v>
@@ -2357,13 +2358,13 @@
         <v>47</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>129</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>154</v>
@@ -2911,11 +2912,11 @@
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">COUNTIF(E2:E67,1)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H69" s="1" t="n">
         <f aca="false">SUMIF(E2:E67,1,H2:H67)+75</f>
-        <v>502</v>
+        <v>518</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,11 +2925,11 @@
       </c>
       <c r="E70" s="0" t="n">
         <f aca="false">E69/E68</f>
-        <v>0.424242424242424</v>
+        <v>0.439393939393939</v>
       </c>
       <c r="H70" s="0" t="n">
         <f aca="false">H69/H68</f>
-        <v>0.422203532380151</v>
+        <v>0.435660218671152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2C0 casi terminado (revisar metadatos)
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -15,17 +15,18 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -123,6 +124,9 @@
     <t xml:space="preserve">Josué</t>
   </si>
   <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
     <t xml:space="preserve">Joshua</t>
   </si>
   <si>
@@ -496,9 +500,6 @@
   </si>
   <si>
     <t xml:space="preserve">2 Corintios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">2 Corinthians</t>
@@ -1050,8 +1051,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1237,11 +1238,14 @@
       <c r="D7" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E7" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="F7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>24</v>
@@ -1258,16 +1262,16 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>21</v>
@@ -1284,7 +1288,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>10</v>
@@ -1293,10 +1297,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>4</v>
@@ -1313,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>10</v>
@@ -1322,10 +1326,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>31</v>
@@ -1342,7 +1346,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>10</v>
@@ -1351,10 +1355,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>24</v>
@@ -1371,16 +1375,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>22</v>
@@ -1397,16 +1401,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>25</v>
@@ -1423,16 +1427,16 @@
         <v>13</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>29</v>
@@ -1449,16 +1453,16 @@
         <v>14</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>36</v>
@@ -1475,16 +1479,16 @@
         <v>15</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>10</v>
@@ -1501,16 +1505,16 @@
         <v>16</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>13</v>
@@ -1527,16 +1531,16 @@
         <v>17</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>10</v>
@@ -1553,7 +1557,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>10</v>
@@ -1562,16 +1566,16 @@
         <v>1</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>42</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1582,7 +1586,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>10</v>
@@ -1591,16 +1595,16 @@
         <v>0.5</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>150</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,22 +1615,22 @@
         <v>20</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>31</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1637,7 +1641,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>10</v>
@@ -1646,16 +1650,16 @@
         <v>1</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>12</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,22 +1670,22 @@
         <v>22</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>8</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,22 +1696,22 @@
         <v>23</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>66</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1718,22 +1722,22 @@
         <v>24</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>52</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,22 +1748,22 @@
         <v>25</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,7 +1774,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>10</v>
@@ -1779,16 +1783,16 @@
         <v>1</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>48</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,22 +1803,22 @@
         <v>27</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>12</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,22 +1829,22 @@
         <v>28</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>14</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,22 +1855,22 @@
         <v>29</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,22 +1881,22 @@
         <v>30</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>9</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,22 +1907,22 @@
         <v>31</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,7 +1933,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>10</v>
@@ -1938,10 +1942,10 @@
         <v>1</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>4</v>
@@ -1958,7 +1962,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>10</v>
@@ -1967,16 +1971,16 @@
         <v>1</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>7</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,7 +1991,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>10</v>
@@ -1996,16 +2000,16 @@
         <v>1</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,7 +2020,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>10</v>
@@ -2025,16 +2029,16 @@
         <v>1</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,7 +2049,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>10</v>
@@ -2054,16 +2058,16 @@
         <v>1</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2074,7 +2078,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>10</v>
@@ -2083,16 +2087,16 @@
         <v>1</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2103,7 +2107,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>10</v>
@@ -2112,16 +2116,16 @@
         <v>1</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>14</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2132,7 +2136,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>10</v>
@@ -2141,16 +2145,16 @@
         <v>1</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>4</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,25 +2165,25 @@
         <v>40</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>28</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2190,22 +2194,22 @@
         <v>41</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H42" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,22 +2220,22 @@
         <v>42</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H43" s="0" t="n">
         <v>24</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,25 +2246,25 @@
         <v>43</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H44" s="0" t="n">
         <v>21</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2271,25 +2275,25 @@
         <v>44</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H45" s="0" t="n">
         <v>28</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2300,25 +2304,25 @@
         <v>45</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H46" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,25 +2333,25 @@
         <v>46</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H47" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,13 +2362,13 @@
         <v>47</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>153</v>
+        <v>130</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>154</v>
@@ -2376,7 +2380,7 @@
         <v>13</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2390,7 +2394,7 @@
         <v>156</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>157</v>
@@ -2402,7 +2406,7 @@
         <v>6</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2416,7 +2420,7 @@
         <v>159</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>160</v>
@@ -2428,7 +2432,7 @@
         <v>6</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2442,7 +2446,7 @@
         <v>162</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>163</v>
@@ -2454,7 +2458,7 @@
         <v>4</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2468,7 +2472,7 @@
         <v>165</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>166</v>
@@ -2480,7 +2484,7 @@
         <v>4</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2494,7 +2498,7 @@
         <v>168</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>169</v>
@@ -2506,7 +2510,7 @@
         <v>5</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,7 +2524,7 @@
         <v>171</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>172</v>
@@ -2532,7 +2536,7 @@
         <v>3</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,7 +2550,7 @@
         <v>174</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>175</v>
@@ -2558,7 +2562,7 @@
         <v>6</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,7 +2576,7 @@
         <v>177</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>178</v>
@@ -2584,7 +2588,7 @@
         <v>4</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,7 +2602,7 @@
         <v>180</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>181</v>
@@ -2610,7 +2614,7 @@
         <v>3</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2624,7 +2628,7 @@
         <v>183</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>184</v>
@@ -2636,7 +2640,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2650,7 +2654,7 @@
         <v>186</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F59" s="0" t="s">
         <v>187</v>
@@ -2662,7 +2666,7 @@
         <v>13</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2676,7 +2680,7 @@
         <v>189</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>1</v>
@@ -2691,7 +2695,7 @@
         <v>5</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,7 +2709,7 @@
         <v>192</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>1</v>
@@ -2720,7 +2724,7 @@
         <v>5</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2734,7 +2738,7 @@
         <v>195</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>1</v>
@@ -2749,7 +2753,7 @@
         <v>3</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2763,7 +2767,7 @@
         <v>198</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>1</v>
@@ -2778,7 +2782,7 @@
         <v>5</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2792,7 +2796,7 @@
         <v>201</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>1</v>
@@ -2807,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2821,7 +2825,7 @@
         <v>204</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>1</v>
@@ -2836,7 +2840,7 @@
         <v>1</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2850,7 +2854,7 @@
         <v>207</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>1</v>
@@ -2865,7 +2869,7 @@
         <v>1</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2879,7 +2883,7 @@
         <v>210</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>1</v>
@@ -2894,7 +2898,7 @@
         <v>22</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2912,11 +2916,11 @@
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">COUNTIF(E2:E67,1)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H69" s="1" t="n">
         <f aca="false">SUMIF(E2:E67,1,H2:H67)+75</f>
-        <v>518</v>
+        <v>531</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2925,11 +2929,11 @@
       </c>
       <c r="E70" s="0" t="n">
         <f aca="false">E69/E68</f>
-        <v>0.439393939393939</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="H70" s="0" t="n">
         <f aca="false">H69/H68</f>
-        <v>0.435660218671152</v>
+        <v>0.44659377628259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Josué terminado e integrado
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -17,17 +17,18 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -125,325 +126,325 @@
     <t xml:space="preserve">Josué</t>
   </si>
   <si>
+    <t xml:space="preserve">Joshua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jueces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Samuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Samuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Reyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Kings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1KI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Reyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Kings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2KI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Crónicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Chronicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Crónicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Chronicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esdras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ezra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EZR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nehemías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nehemiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wisdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psalms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lyric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proverbios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proverbs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eclesiastés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecclesiastes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Song of Solomon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apocalyptic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeremías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeremiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prophecy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lamentaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lamentations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ezequiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ezekiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oseas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hosea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amós</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obadiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miqueas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nahúm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nahum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habacuc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habakkuk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofonías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zephaniah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hageo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haggai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zacarías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zechariah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malaquías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malachi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mateo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuevo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matthew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gospel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcos</t>
+  </si>
+  <si>
     <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joshua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jueces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Judges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JDG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Samuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1SA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Samuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2SA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Reyes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Kings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1KI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Reyes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Kings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2KI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Crónicas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Chronicles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Crónicas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Chronicles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esdras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ezra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EZR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nehemías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nehemiah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Job</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wisdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psalms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lyric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proverbios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proverbs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eclesiastés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecclesiastes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cantares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Song of Solomon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isaías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isaiah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">apocalyptic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeremías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeremiah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prophecy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lamentaciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lamentations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ezequiel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ezekiel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EZE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oseas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hosea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amós</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abdías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Obadiah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OBA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jonás</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jonah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miqueas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nahúm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nahum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Habacuc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Habakkuk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sofonías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zephaniah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hageo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haggai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zacarías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zechariah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZEC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malaquías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malachi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mateo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nuevo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matthew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gospel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marcos</t>
   </si>
   <si>
     <t xml:space="preserve">Mark</t>
@@ -1052,8 +1053,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H71" activeCellId="0" sqref="H71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1239,14 +1240,14 @@
       <c r="D7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>24</v>
@@ -1263,16 +1264,16 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>21</v>
@@ -1289,19 +1290,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>4</v>
@@ -1318,19 +1319,19 @@
         <v>9</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>31</v>
@@ -1347,19 +1348,19 @@
         <v>10</v>
       </c>
       <c r="C11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>24</v>
@@ -1376,16 +1377,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="G12" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>22</v>
@@ -1402,16 +1403,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>46</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>25</v>
@@ -1428,16 +1429,16 @@
         <v>13</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>29</v>
@@ -1454,16 +1455,16 @@
         <v>14</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="0" t="s">
+      <c r="G15" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>36</v>
@@ -1480,16 +1481,16 @@
         <v>15</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="0" t="s">
+      <c r="G16" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>10</v>
@@ -1506,16 +1507,16 @@
         <v>16</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="G17" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>13</v>
@@ -1532,16 +1533,16 @@
         <v>17</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="G18" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>61</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>10</v>
@@ -1558,25 +1559,25 @@
         <v>18</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>63</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>42</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,7 +1588,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>10</v>
@@ -1596,16 +1597,16 @@
         <v>0.5</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>150</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,22 +1617,22 @@
         <v>20</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="0" t="s">
+      <c r="G21" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>71</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>31</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,25 +1643,25 @@
         <v>21</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="0" t="s">
+      <c r="G22" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>74</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>12</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,22 +1672,22 @@
         <v>22</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="0" t="s">
+      <c r="G23" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>8</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1697,22 +1698,22 @@
         <v>23</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="0" t="s">
+      <c r="G24" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>66</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1723,22 +1724,22 @@
         <v>24</v>
       </c>
       <c r="C25" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="0" t="s">
+      <c r="G25" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>84</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>52</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,22 +1750,22 @@
         <v>25</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="0" t="s">
+      <c r="G26" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>88</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,25 +1776,25 @@
         <v>26</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F27" s="0" t="s">
+      <c r="G27" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>48</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,22 +1805,22 @@
         <v>27</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>12</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,22 +1831,22 @@
         <v>28</v>
       </c>
       <c r="C29" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="0" t="s">
+      <c r="G29" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>14</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,22 +1857,22 @@
         <v>29</v>
       </c>
       <c r="C30" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,22 +1883,22 @@
         <v>30</v>
       </c>
       <c r="C31" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="0" t="s">
+      <c r="G31" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>9</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,22 +1909,22 @@
         <v>31</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="0" t="s">
+      <c r="G32" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="0" t="s">
-        <v>104</v>
-      </c>
       <c r="H32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,19 +1935,19 @@
         <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F33" s="0" t="s">
+      <c r="G33" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>4</v>
@@ -1963,25 +1964,25 @@
         <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="0" t="s">
+      <c r="G34" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>7</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,25 +1993,25 @@
         <v>34</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F35" s="0" t="s">
+      <c r="G35" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2021,25 +2022,25 @@
         <v>35</v>
       </c>
       <c r="C36" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F36" s="0" t="s">
+      <c r="G36" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>116</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,25 +2051,25 @@
         <v>36</v>
       </c>
       <c r="C37" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F37" s="0" t="s">
+      <c r="G37" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>119</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,25 +2080,25 @@
         <v>37</v>
       </c>
       <c r="C38" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F38" s="0" t="s">
+      <c r="G38" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>122</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,25 +2109,25 @@
         <v>38</v>
       </c>
       <c r="C39" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F39" s="0" t="s">
+      <c r="G39" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>125</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>14</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2137,25 +2138,25 @@
         <v>39</v>
       </c>
       <c r="C40" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F40" s="0" t="s">
+      <c r="G40" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>128</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>4</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,25 +2167,25 @@
         <v>40</v>
       </c>
       <c r="C41" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="E41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="E41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" s="0" t="s">
+      <c r="G41" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>132</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>28</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2195,10 +2196,13 @@
         <v>41</v>
       </c>
       <c r="C42" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>130</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>135</v>
@@ -2210,7 +2214,7 @@
         <v>16</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,7 +2228,7 @@
         <v>137</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>138</v>
@@ -2236,7 +2240,7 @@
         <v>24</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,7 +2254,7 @@
         <v>140</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>1</v>
@@ -2265,7 +2269,7 @@
         <v>21</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2279,7 +2283,7 @@
         <v>143</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>1</v>
@@ -2294,7 +2298,7 @@
         <v>28</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,7 +2312,7 @@
         <v>146</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>1</v>
@@ -2337,7 +2341,7 @@
         <v>150</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>1</v>
@@ -2366,7 +2370,7 @@
         <v>153</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>1</v>
@@ -2395,7 +2399,7 @@
         <v>156</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>157</v>
@@ -2421,7 +2425,7 @@
         <v>159</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>160</v>
@@ -2447,7 +2451,7 @@
         <v>162</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>163</v>
@@ -2473,7 +2477,7 @@
         <v>165</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>166</v>
@@ -2499,7 +2503,7 @@
         <v>168</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>169</v>
@@ -2525,7 +2529,7 @@
         <v>171</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>172</v>
@@ -2551,7 +2555,7 @@
         <v>174</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>175</v>
@@ -2577,7 +2581,7 @@
         <v>177</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>178</v>
@@ -2603,7 +2607,7 @@
         <v>180</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>181</v>
@@ -2629,7 +2633,7 @@
         <v>183</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>184</v>
@@ -2655,7 +2659,7 @@
         <v>186</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F59" s="0" t="s">
         <v>187</v>
@@ -2681,7 +2685,7 @@
         <v>189</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>1</v>
@@ -2710,7 +2714,7 @@
         <v>192</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>1</v>
@@ -2739,7 +2743,7 @@
         <v>195</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>1</v>
@@ -2768,7 +2772,7 @@
         <v>198</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>1</v>
@@ -2797,7 +2801,7 @@
         <v>201</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>1</v>
@@ -2826,7 +2830,7 @@
         <v>204</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>1</v>
@@ -2855,7 +2859,7 @@
         <v>207</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>1</v>
@@ -2884,7 +2888,7 @@
         <v>210</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>1</v>
@@ -2899,7 +2903,7 @@
         <v>22</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,11 +2921,11 @@
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">COUNTIF(E2:E67,1)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H69" s="1" t="n">
         <f aca="false">SUMIF(E2:E67,1,H2:H67)+75</f>
-        <v>531</v>
+        <v>555</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2930,11 +2934,11 @@
       </c>
       <c r="E70" s="0" t="n">
         <f aca="false">E69/E68</f>
-        <v>0.454545454545455</v>
+        <v>0.46969696969697</v>
       </c>
       <c r="H70" s="0" t="n">
         <f aca="false">H69/H68</f>
-        <v>0.44659377628259</v>
+        <v>0.466778805719092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oseas terminado y archivos gefx de networks de libros
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -22,17 +22,18 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="214">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -326,9 +327,6 @@
   </si>
   <si>
     <t xml:space="preserve">Oseas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">Hosea</t>
@@ -1066,8 +1064,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1862,14 +1860,14 @@
       <c r="D29" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="G29" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>14</v>
@@ -1886,16 +1884,16 @@
         <v>29</v>
       </c>
       <c r="C30" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>3</v>
@@ -1912,16 +1910,16 @@
         <v>30</v>
       </c>
       <c r="C31" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="0" t="s">
+      <c r="G31" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>9</v>
@@ -1938,16 +1936,16 @@
         <v>31</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="0" t="s">
+      <c r="G32" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>104</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>1</v>
@@ -1964,19 +1962,19 @@
         <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F33" s="0" t="s">
+      <c r="G33" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>4</v>
@@ -1993,19 +1991,19 @@
         <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="0" t="s">
+      <c r="G34" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>7</v>
@@ -2022,19 +2020,19 @@
         <v>34</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F35" s="0" t="s">
+      <c r="G35" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>3</v>
@@ -2051,19 +2049,19 @@
         <v>35</v>
       </c>
       <c r="C36" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F36" s="0" t="s">
+      <c r="G36" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>116</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>3</v>
@@ -2080,19 +2078,19 @@
         <v>36</v>
       </c>
       <c r="C37" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F37" s="0" t="s">
+      <c r="G37" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>119</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>3</v>
@@ -2109,19 +2107,19 @@
         <v>37</v>
       </c>
       <c r="C38" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F38" s="0" t="s">
+      <c r="G38" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>122</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>2</v>
@@ -2138,19 +2136,19 @@
         <v>38</v>
       </c>
       <c r="C39" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F39" s="0" t="s">
+      <c r="G39" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>125</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>14</v>
@@ -2167,19 +2165,19 @@
         <v>39</v>
       </c>
       <c r="C40" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F40" s="0" t="s">
+      <c r="G40" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>128</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>4</v>
@@ -2196,25 +2194,25 @@
         <v>40</v>
       </c>
       <c r="C41" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="E41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="E41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" s="0" t="s">
+      <c r="G41" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>132</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>28</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,25 +2223,25 @@
         <v>41</v>
       </c>
       <c r="C42" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F42" s="0" t="s">
+      <c r="G42" s="0" t="s">
         <v>135</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>136</v>
       </c>
       <c r="H42" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,22 +2252,22 @@
         <v>42</v>
       </c>
       <c r="C43" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F43" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F43" s="0" t="s">
+      <c r="G43" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>139</v>
       </c>
       <c r="H43" s="0" t="n">
         <v>24</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,25 +2278,25 @@
         <v>43</v>
       </c>
       <c r="C44" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F44" s="0" t="s">
+      <c r="G44" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>142</v>
       </c>
       <c r="H44" s="0" t="n">
         <v>21</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2309,25 +2307,25 @@
         <v>44</v>
       </c>
       <c r="C45" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F45" s="0" t="s">
+      <c r="G45" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>145</v>
       </c>
       <c r="H45" s="0" t="n">
         <v>28</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,25 +2336,25 @@
         <v>45</v>
       </c>
       <c r="C46" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F46" s="0" t="s">
+      <c r="G46" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="G46" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="H46" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,25 +2365,25 @@
         <v>46</v>
       </c>
       <c r="C47" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F47" s="0" t="s">
+      <c r="G47" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>152</v>
       </c>
       <c r="H47" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,25 +2394,25 @@
         <v>47</v>
       </c>
       <c r="C48" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F48" s="0" t="s">
+      <c r="G48" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="G48" s="0" t="s">
-        <v>155</v>
       </c>
       <c r="H48" s="0" t="n">
         <v>13</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,22 +2423,22 @@
         <v>48</v>
       </c>
       <c r="C49" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F49" s="0" t="s">
+      <c r="G49" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>158</v>
       </c>
       <c r="H49" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,22 +2449,22 @@
         <v>49</v>
       </c>
       <c r="C50" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F50" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F50" s="0" t="s">
+      <c r="G50" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>161</v>
       </c>
       <c r="H50" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2477,22 +2475,22 @@
         <v>50</v>
       </c>
       <c r="C51" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F51" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F51" s="0" t="s">
+      <c r="G51" s="0" t="s">
         <v>163</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>164</v>
       </c>
       <c r="H51" s="0" t="n">
         <v>4</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2503,22 +2501,22 @@
         <v>51</v>
       </c>
       <c r="C52" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F52" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F52" s="0" t="s">
+      <c r="G52" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="H52" s="0" t="n">
         <v>4</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2529,22 +2527,22 @@
         <v>52</v>
       </c>
       <c r="C53" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F53" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="D53" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F53" s="0" t="s">
+      <c r="G53" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="H53" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2555,22 +2553,22 @@
         <v>53</v>
       </c>
       <c r="C54" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F54" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="D54" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F54" s="0" t="s">
+      <c r="G54" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="G54" s="0" t="s">
-        <v>173</v>
       </c>
       <c r="H54" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2581,22 +2579,22 @@
         <v>54</v>
       </c>
       <c r="C55" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F55" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="D55" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F55" s="0" t="s">
+      <c r="G55" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="G55" s="0" t="s">
-        <v>176</v>
       </c>
       <c r="H55" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2607,22 +2605,22 @@
         <v>55</v>
       </c>
       <c r="C56" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F56" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="D56" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F56" s="0" t="s">
+      <c r="G56" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="G56" s="0" t="s">
-        <v>179</v>
       </c>
       <c r="H56" s="0" t="n">
         <v>4</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2633,22 +2631,22 @@
         <v>56</v>
       </c>
       <c r="C57" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F57" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="D57" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F57" s="0" t="s">
+      <c r="G57" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="G57" s="0" t="s">
-        <v>182</v>
       </c>
       <c r="H57" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2659,22 +2657,22 @@
         <v>57</v>
       </c>
       <c r="C58" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F58" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F58" s="0" t="s">
+      <c r="G58" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="G58" s="0" t="s">
-        <v>185</v>
-      </c>
       <c r="H58" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,22 +2683,22 @@
         <v>58</v>
       </c>
       <c r="C59" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F59" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F59" s="0" t="s">
+      <c r="G59" s="0" t="s">
         <v>187</v>
-      </c>
-      <c r="G59" s="0" t="s">
-        <v>188</v>
       </c>
       <c r="H59" s="0" t="n">
         <v>13</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2711,25 +2709,25 @@
         <v>59</v>
       </c>
       <c r="C60" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="D60" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E60" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F60" s="0" t="s">
+      <c r="G60" s="0" t="s">
         <v>190</v>
-      </c>
-      <c r="G60" s="0" t="s">
-        <v>191</v>
       </c>
       <c r="H60" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2740,25 +2738,25 @@
         <v>60</v>
       </c>
       <c r="C61" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="D61" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E61" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F61" s="0" t="s">
+      <c r="G61" s="0" t="s">
         <v>193</v>
-      </c>
-      <c r="G61" s="0" t="s">
-        <v>194</v>
       </c>
       <c r="H61" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2769,25 +2767,25 @@
         <v>61</v>
       </c>
       <c r="C62" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="D62" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E62" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F62" s="0" t="s">
+      <c r="G62" s="0" t="s">
         <v>196</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>197</v>
       </c>
       <c r="H62" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,25 +2796,25 @@
         <v>62</v>
       </c>
       <c r="C63" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E63" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F63" s="0" t="s">
+      <c r="G63" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="G63" s="0" t="s">
-        <v>200</v>
       </c>
       <c r="H63" s="0" t="n">
         <v>5</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2827,25 +2825,25 @@
         <v>63</v>
       </c>
       <c r="C64" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="D64" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E64" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F64" s="0" t="s">
+      <c r="G64" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="G64" s="0" t="s">
-        <v>203</v>
-      </c>
       <c r="H64" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2856,25 +2854,25 @@
         <v>64</v>
       </c>
       <c r="C65" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F65" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="D65" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E65" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F65" s="0" t="s">
+      <c r="G65" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="G65" s="0" t="s">
-        <v>206</v>
-      </c>
       <c r="H65" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2885,25 +2883,25 @@
         <v>65</v>
       </c>
       <c r="C66" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="D66" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F66" s="0" t="s">
+      <c r="G66" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="G66" s="0" t="s">
-        <v>209</v>
-      </c>
       <c r="H66" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2914,19 +2912,19 @@
         <v>66</v>
       </c>
       <c r="C67" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F67" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="D67" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E67" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F67" s="0" t="s">
+      <c r="G67" s="0" t="s">
         <v>211</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>212</v>
       </c>
       <c r="H67" s="0" t="n">
         <v>22</v>
@@ -2946,30 +2944,30 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D69" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">COUNTIF(E2:E67,1)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H69" s="1" t="n">
         <f aca="false">SUMIF(E2:E67,1,H2:H67)+75</f>
-        <v>583</v>
+        <v>597</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D70" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E70" s="3" t="n">
         <f aca="false">E69/E68</f>
-        <v>0.5</v>
+        <v>0.515151515151515</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3" t="n">
         <f aca="false">H69/H68</f>
-        <v>0.490328006728343</v>
+        <v>0.502102607232969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nueva función para dividirBiblia en libros
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -27,17 +27,18 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -1071,8 +1072,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
script a TEI mejorado
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -28,17 +28,18 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -1067,13 +1068,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1119,7 +1120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>0</v>
       </c>
@@ -1255,7 +1256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1285,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>0</v>
       </c>
@@ -1342,7 +1343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>0</v>
       </c>
@@ -1371,7 +1372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>0</v>
       </c>
@@ -1530,7 +1531,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>0</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>0</v>
       </c>
@@ -1669,7 +1670,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>0</v>
       </c>
@@ -1802,7 +1803,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>0</v>
       </c>
@@ -1831,7 +1832,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>0</v>
       </c>
@@ -1860,7 +1861,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>0</v>
       </c>
@@ -1941,7 +1942,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>0</v>
       </c>
@@ -1970,7 +1971,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>0</v>
       </c>
@@ -1999,7 +2000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>0</v>
       </c>
@@ -2028,7 +2029,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>0</v>
       </c>
@@ -2057,7 +2058,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>0</v>
       </c>
@@ -2086,7 +2087,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>0</v>
       </c>
@@ -2115,7 +2116,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>0</v>
       </c>
@@ -2144,7 +2145,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>0</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>0</v>
       </c>
@@ -2202,7 +2203,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>0</v>
       </c>
@@ -2231,7 +2232,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>0</v>
       </c>
@@ -2286,7 +2287,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>0</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>0</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>0</v>
       </c>
@@ -2373,7 +2374,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>0</v>
       </c>
@@ -2402,7 +2403,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>0</v>
       </c>
@@ -2717,7 +2718,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>0</v>
       </c>
@@ -2746,7 +2747,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>0</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>0</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>0</v>
       </c>
@@ -2833,7 +2834,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>0</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>0</v>
       </c>
@@ -2891,7 +2892,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>0</v>
       </c>
@@ -2920,7 +2921,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>0</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="0" t="n">
         <v>66</v>
       </c>
@@ -2958,7 +2959,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D69" s="0" t="s">
         <v>213</v>
       </c>
@@ -2971,7 +2972,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D70" s="0" t="s">
         <v>214</v>
       </c>
@@ -2987,7 +2988,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:I70"/>
+  <autoFilter ref="B1:I70">
+    <filterColumn colId="3">
+      <customFilters and="true">
+        <customFilter operator="equal" val="0"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Changes in documentation of books
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
@@ -30,17 +30,19 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="216">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -697,6 +699,9 @@
   </si>
   <si>
     <t xml:space="preserve">proportion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total falta</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1077,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1192,6 +1197,9 @@
       <c r="D4" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F4" s="0" t="s">
         <v>18</v>
       </c>
@@ -1218,6 +1226,9 @@
       <c r="D5" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F5" s="0" t="s">
         <v>22</v>
       </c>
@@ -1244,6 +1255,9 @@
       <c r="D6" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F6" s="0" t="s">
         <v>25</v>
       </c>
@@ -1415,6 +1429,9 @@
       <c r="D12" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F12" s="0" t="s">
         <v>41</v>
       </c>
@@ -1441,6 +1458,9 @@
       <c r="D13" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E13" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F13" s="0" t="s">
         <v>44</v>
       </c>
@@ -1467,6 +1487,9 @@
       <c r="D14" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F14" s="0" t="s">
         <v>47</v>
       </c>
@@ -1493,6 +1516,9 @@
       <c r="D15" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E15" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F15" s="0" t="s">
         <v>50</v>
       </c>
@@ -1519,6 +1545,9 @@
       <c r="D16" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F16" s="0" t="s">
         <v>53</v>
       </c>
@@ -1574,6 +1603,9 @@
       <c r="D18" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F18" s="0" t="s">
         <v>60</v>
       </c>
@@ -1658,6 +1690,9 @@
       <c r="D21" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F21" s="0" t="s">
         <v>70</v>
       </c>
@@ -1713,6 +1748,9 @@
       <c r="D23" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F23" s="0" t="s">
         <v>76</v>
       </c>
@@ -1739,6 +1777,9 @@
       <c r="D24" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F24" s="0" t="s">
         <v>79</v>
       </c>
@@ -1765,6 +1806,9 @@
       <c r="D25" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F25" s="0" t="s">
         <v>83</v>
       </c>
@@ -1791,6 +1835,9 @@
       <c r="D26" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F26" s="0" t="s">
         <v>87</v>
       </c>
@@ -1933,6 +1980,9 @@
       <c r="D31" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F31" s="0" t="s">
         <v>100</v>
       </c>
@@ -2278,6 +2328,9 @@
       <c r="D43" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E43" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F43" s="0" t="s">
         <v>138</v>
       </c>
@@ -2449,6 +2502,9 @@
       <c r="D49" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E49" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F49" s="0" t="s">
         <v>157</v>
       </c>
@@ -2475,6 +2531,9 @@
       <c r="D50" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E50" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F50" s="0" t="s">
         <v>160</v>
       </c>
@@ -2501,6 +2560,9 @@
       <c r="D51" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E51" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F51" s="0" t="s">
         <v>163</v>
       </c>
@@ -2527,6 +2589,9 @@
       <c r="D52" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E52" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F52" s="0" t="s">
         <v>166</v>
       </c>
@@ -2553,6 +2618,9 @@
       <c r="D53" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E53" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F53" s="0" t="s">
         <v>169</v>
       </c>
@@ -2579,6 +2647,9 @@
       <c r="D54" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E54" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F54" s="0" t="s">
         <v>172</v>
       </c>
@@ -2605,6 +2676,9 @@
       <c r="D55" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E55" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F55" s="0" t="s">
         <v>175</v>
       </c>
@@ -2631,6 +2705,9 @@
       <c r="D56" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E56" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F56" s="0" t="s">
         <v>178</v>
       </c>
@@ -2657,6 +2734,9 @@
       <c r="D57" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E57" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F57" s="0" t="s">
         <v>181</v>
       </c>
@@ -2683,6 +2763,9 @@
       <c r="D58" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E58" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F58" s="0" t="s">
         <v>184</v>
       </c>
@@ -2708,6 +2791,9 @@
       </c>
       <c r="D59" s="0" t="s">
         <v>130</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="F59" s="0" t="s">
         <v>187</v>
@@ -2989,6 +3075,19 @@
       <c r="H70" s="3" t="n">
         <f aca="false">H69/H68</f>
         <v>0.523128679562658</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D71" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E69,0)</f>
+        <v>27</v>
+      </c>
+      <c r="H71" s="1" t="n">
+        <f aca="false">SUMIF(E2:E67,0,H2:H67)+75</f>
+        <v>554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Esdras integrado en archivo principal
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -14,11 +14,11 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
@@ -37,17 +37,18 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -1091,7 +1092,7 @@
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1557,7 +1558,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>53</v>
@@ -3066,11 +3067,11 @@
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">COUNTIF(E2:E67,1)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H69" s="1" t="n">
         <f aca="false">SUMIF(E2:E67,1,H2:H67)+75</f>
-        <v>786</v>
+        <v>796</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3079,13 +3080,13 @@
       </c>
       <c r="E70" s="3" t="n">
         <f aca="false">E69/E68</f>
-        <v>0.606060606060606</v>
+        <v>0.621212121212121</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3" t="n">
         <f aca="false">H69/H68</f>
-        <v>0.661059714045416</v>
+        <v>0.669470142977292</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3094,11 +3095,11 @@
       </c>
       <c r="E71" s="0" t="n">
         <f aca="false">COUNTIF(E2:E69,0)</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H71" s="1" t="n">
         <f aca="false">SUMIF(E2:E67,0,H2:H67)+75</f>
-        <v>553</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Empezando 1 y 2 de Timoteo y Tito
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -15,12 +15,12 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
@@ -38,17 +38,19 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="219">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -582,6 +584,9 @@
   </si>
   <si>
     <t xml:space="preserve">1 Timoteo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">1 Timothy</t>
@@ -1091,8 +1096,8 @@
   </sheetPr>
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D62" activeCellId="0" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2688,14 +2693,14 @@
       <c r="D55" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E55" s="0" t="n">
-        <v>0</v>
+      <c r="E55" s="0" t="s">
+        <v>174</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H55" s="0" t="n">
         <v>6</v>
@@ -2712,19 +2717,19 @@
         <v>55</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E56" s="0" t="n">
-        <v>0</v>
+      <c r="E56" s="0" t="s">
+        <v>174</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H56" s="0" t="n">
         <v>4</v>
@@ -2741,19 +2746,19 @@
         <v>56</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E57" s="0" t="n">
-        <v>0</v>
+      <c r="E57" s="0" t="s">
+        <v>174</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H57" s="0" t="n">
         <v>3</v>
@@ -2770,7 +2775,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>129</v>
@@ -2779,10 +2784,10 @@
         <v>1</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H58" s="0" t="n">
         <v>1</v>
@@ -2799,7 +2804,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>129</v>
@@ -2808,10 +2813,10 @@
         <v>0</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H59" s="0" t="n">
         <v>13</v>
@@ -2828,7 +2833,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>129</v>
@@ -2837,10 +2842,10 @@
         <v>1</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H60" s="0" t="n">
         <v>5</v>
@@ -2857,7 +2862,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>129</v>
@@ -2866,10 +2871,10 @@
         <v>1</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H61" s="0" t="n">
         <v>5</v>
@@ -2886,7 +2891,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>129</v>
@@ -2895,10 +2900,10 @@
         <v>1</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H62" s="0" t="n">
         <v>3</v>
@@ -2915,7 +2920,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>129</v>
@@ -2924,10 +2929,10 @@
         <v>1</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H63" s="0" t="n">
         <v>5</v>
@@ -2944,7 +2949,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>129</v>
@@ -2953,10 +2958,10 @@
         <v>1</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H64" s="0" t="n">
         <v>1</v>
@@ -2973,7 +2978,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>129</v>
@@ -2982,10 +2987,10 @@
         <v>1</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H65" s="0" t="n">
         <v>1</v>
@@ -3002,7 +3007,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>129</v>
@@ -3011,10 +3016,10 @@
         <v>1</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H66" s="0" t="n">
         <v>1</v>
@@ -3031,7 +3036,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>129</v>
@@ -3040,10 +3045,10 @@
         <v>1</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H67" s="0" t="n">
         <v>22</v>
@@ -3063,7 +3068,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D69" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">COUNTIF(E2:E67,1)</f>
@@ -3076,7 +3081,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D70" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E70" s="3" t="n">
         <f aca="false">E69/E68</f>
@@ -3091,15 +3096,15 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D71" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E71" s="0" t="n">
         <f aca="false">COUNTIF(E2:E69,0)</f>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H71" s="1" t="n">
         <f aca="false">SUMIF(E2:E67,0,H2:H67)+75</f>
-        <v>543</v>
+        <v>530</v>
       </c>
     </row>
   </sheetData>
@@ -3133,7 +3138,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B2" s="3" t="n">
         <f aca="false">AVERAGE(Sheet1!$H$2:$H$67)</f>
@@ -3142,7 +3147,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B3" s="3" t="n">
         <f aca="false">MEDIAN(Sheet1!$H$2:$H$67)</f>
@@ -3151,7 +3156,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B4" s="3" t="n">
         <f aca="false">STDEV(Sheet1!$H$2:$H$67)</f>

</xml_diff>

<commit_message>
Capítulo 1 de timoteo corregido
</commit_message>
<xml_diff>
--- a/documentation/libros.xlsx
+++ b/documentation/libros.xlsx
@@ -17,11 +17,11 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
@@ -40,17 +40,18 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -1097,7 +1098,7 @@
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D62" activeCellId="0" sqref="D62"/>
+      <selection pane="topLeft" activeCell="F57" activeCellId="0" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>